<commit_message>
update the worksheets attached
</commit_message>
<xml_diff>
--- a/Payroll System_v3.xlsx
+++ b/Payroll System_v3.xlsx
@@ -40,6 +40,11 @@
     <comment authorId="0" ref="D1">
       <text>
         <t xml:space="preserve">Weekly OT starts after first threshold hours</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E1">
+      <text>
+        <t xml:space="preserve">Enable/Disable Parsing Weekend Early/Late Over Time</t>
       </text>
     </comment>
   </commentList>
@@ -105,6 +110,12 @@
     <comment authorId="0" ref="K1">
       <text>
         <t xml:space="preserve">Wage after closing hours (Sunday)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="L1">
+      <text>
+        <t xml:space="preserve">Enable/Disable show wage 
+calculation</t>
       </text>
     </comment>
   </commentList>
@@ -586,6 +597,419 @@
     </xdr:sp>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3514725" cy="5457825"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Shape 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1471875" y="263925"/>
+          <a:ext cx="3492000" cy="5715000"/>
+        </a:xfrm>
+        <a:prstGeom prst="foldedCorner">
+          <a:avLst>
+            <a:gd fmla="val 16667" name="adj"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFF2CC"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1400"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300"/>
+            <a:t>How to Use This Sheet</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1300"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buAutoNum type="arabicPeriod"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Enter your </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Date, Name, Shift Start Time, Shift End Time, and Break (hours)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> from the Work Log.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buAutoNum type="arabicPeriod"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Click the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Generate Payslip</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> button to run the script.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The script will calculate work hours based on your time policy and create weekly payslips in the sheet </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>“Payslip List”</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>You can print the payslips if required.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buAutoNum type="arabicPeriod"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Before entering a new week’s Work Log, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>delete all previous records</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1400"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300"/>
+            <a:t>Important Warnings</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1300"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Do not delete or modify the header row.</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Keep column formats consistent:</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>Date</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>Start Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>End Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> → Date/Time format</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>Name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> → Text</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>Break</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> → Numbe</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>r</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If any records fail validation, you will receive a notification.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Invalid entries are </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>excluded</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> from the calculation until corrected.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100"/>
+          </a:br>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -601,7 +1025,7 @@
     <xdr:ext cx="1895475" cy="685800"/>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Shape 4"/>
+        <xdr:cNvPr id="5" name="Shape 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -660,11 +1084,1023 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>-171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4629150" cy="3352800"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Shape 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="375525" y="203025"/>
+          <a:ext cx="4608600" cy="3329400"/>
+        </a:xfrm>
+        <a:prstGeom prst="foldedCorner">
+          <a:avLst>
+            <a:gd fmla="val 16667" name="adj"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFF2CC"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1400"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300"/>
+            <a:t>Time Config Panel</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1300"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This sheet provides the reference settings the script uses to calculate work logs according to your business’s time policy.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Do not edit these values unless you have confirmed a change in business policy.</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1400"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300"/>
+            <a:t>Warnings</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1300"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Never delete or modify the header row.</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If the config fails validation, you will receive a warning and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>calculation will not proceed</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> until fixed.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5915025" cy="5505450"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Shape 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="406050" y="223325"/>
+          <a:ext cx="5897700" cy="5420700"/>
+        </a:xfrm>
+        <a:prstGeom prst="foldedCorner">
+          <a:avLst>
+            <a:gd fmla="val 16667" name="adj"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFF2CC"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1400"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300"/>
+            <a:t>Column Guide</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1300"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>OPEN_TIME / CLOSE_TIME</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> Defines regular business hours.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Any hours outside this range are considered </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>early/late overtime</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Values must be in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Date/Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> format.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>CLOSE_TIME</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> must always be later than </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr i="1" lang="en-US" sz="1100"/>
+            <a:t>OPEN_TIME</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>OT_DAILY_TIME_THRESHOLD / OT_WEEKLY_TIME_THRESHOLD</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> Defines the daily or weekly thresholds for overtime.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If staff work beyond these thresholds, excess hours are assigned higher wage rates.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Example: OT_WEEKLY_TIME_THRESHOLD = 38,40 means hours over 38 and 40 in a week are calculated separately at higher rates.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Values must be either:</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="2" marL="1371600" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="■"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>a single number (e.g. 12), or</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="2" marL="1371600" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="■"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>a comma-separated list without spaces (e.g. 38,42,45).</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Wage Threshold Alignment</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> The number of thresholds must always match the number of wage levels.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Example: if OT_WEEKLY_TIME_THRESHOLD = 38,42,45 then OT_WEEKLY_THRESHOLD_WAGE must also have </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>three elements</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> (e.g. 36.15,37.25,40).</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>BOOL_WEEKEND_OT</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> Enables or disables weekend overtime parsing.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Must be a </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Boolean</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> value: TRUE or FALSE.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If enabled, weekend hours are split into Early OT / Late OT / Regular, instead of being counted entirely as regular hours.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="ctr">
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4210050" cy="2943225"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Shape 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="578575" y="131975"/>
+          <a:ext cx="4192500" cy="2923500"/>
+        </a:xfrm>
+        <a:prstGeom prst="foldedCorner">
+          <a:avLst>
+            <a:gd fmla="val 16667" name="adj"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFF2CC"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1400"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300"/>
+            <a:t>Wage Config Panel</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1300"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This sheet defines the reference settings the script uses to calculate wages for different rates of parsed working hours.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Wage is always calculated in the background.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Wages will only be displayed on payslips if </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>BOOL_SHOW_WAGE = TRUE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you do not require this feature, you can usually ignore this sheet.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Never delete or modify the header row.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4362450" cy="3933825"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Shape 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="314675" y="233475"/>
+          <a:ext cx="4344600" cy="3674700"/>
+        </a:xfrm>
+        <a:prstGeom prst="foldedCorner">
+          <a:avLst>
+            <a:gd fmla="val 16667" name="adj"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFF2CC"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1400"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300"/>
+            <a:t>Key Rules</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1300"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1200"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Threshold–Wage Alignment</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> The number of thresholds must always match the number of wage levels.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Example: if OT_WEEKLY_TIME_THRESHOLD = 38,42,45 then OT_WEEKLY_THRESHOLD_WAGE must also contain three values (e.g. 36.15,37.25,40).</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Break Time Policy</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> Break hours are always deducted from the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>lowest wage rate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> working hours.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="0" marL="457200" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="●"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>Recommended Setup</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> Even if you do not use wage calculation, it is strongly recommended to set up </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1100"/>
+            <a:t>mock salary values</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="-298450" lvl="1" marL="914400" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buSzPts val="1100"/>
+            <a:buChar char="○"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This helps preserve the correct proportional relationship between wage levels.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100"/>
+          </a:br>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>